<commit_message>
You can commit if you want to, you can leave your friends behind
</commit_message>
<xml_diff>
--- a/WeaponStats.xlsx
+++ b/WeaponStats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -435,13 +435,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A329C159-9717-4EF8-9E7F-AA780CE10AF9}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -470,10 +473,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <v>7</v>
@@ -484,10 +487,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>15</v>
@@ -511,170 +514,184 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.72</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.72</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <v>0.433</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>0.86599999999999999</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>1.0329999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="1">
-        <f>PRODUCT(B3,1/B9)</f>
-        <v>10</v>
-      </c>
-      <c r="C15" s="1">
-        <f>PRODUCT(C3,1/C9)</f>
-        <v>8.3333333333333321</v>
-      </c>
-      <c r="D15" s="1">
-        <f>PRODUCT(D3,1/D9)</f>
+      <c r="B17" s="1">
+        <f t="shared" ref="B17:D20" si="0">PRODUCT(B3,1/B10)</f>
+        <v>7.5</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
         <v>9.7222222222222214</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1">
-        <f t="shared" ref="B16:D16" si="0">PRODUCT(B4,1/B10)</f>
-        <v>8.0831408775981526</v>
-      </c>
-      <c r="C16" s="1">
-        <f t="shared" si="0"/>
-        <v>10.392609699769052</v>
-      </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>14.520813165537271</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="1">
-        <f t="shared" ref="B17:D17" si="1">PRODUCT(B5,1/B11)</f>
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" si="1"/>
-        <v>9.1666666666666679</v>
-      </c>
       <c r="D17" s="1">
-        <f t="shared" si="1"/>
-        <v>6.5217391304347823</v>
+        <f t="shared" si="0"/>
+        <v>9.7222222222222214</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>6.9284064665127012</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>11.547344110854503</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>14.520813165537271</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B18" s="1" t="e">
-        <f t="shared" ref="B18:D18" si="2">PRODUCT(B6,1/B12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C18" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D18" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>9.1666666666666679</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>6.5217391304347823</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>